<commit_message>
Trial 1 building functins for rate kinetics
</commit_message>
<xml_diff>
--- a/data/train_data/vegf_testdata/VEGFA165_NRP1_0.5-8nM_Lu2023.xlsx
+++ b/data/train_data/vegf_testdata/VEGFA165_NRP1_0.5-8nM_Lu2023.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lione\Desktop\GitHub\meta-analysis-for-VEGF-signaling\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwnetid-my.sharepoint.com/personal/ltukei_uw_edu/Documents/Desktop/GitHub/Data_extraction_kinetic_signaling_data/data/train_data/vegf_testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D15D483-637D-430C-9692-69D62ACC1FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{6D15D483-637D-430C-9692-69D62ACC1FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C82BCABB-A80A-4D6B-A8C7-09B241BCC0CE}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15360" yWindow="3675" windowWidth="15570" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -202,7 +202,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$39</c:f>
+              <c:f>sheet1!$A$2:$A$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="38"/>
@@ -298,7 +298,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$39</c:f>
+              <c:f>sheet1!$B$2:$B$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="38"/>
@@ -431,7 +431,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$39</c:f>
+              <c:f>sheet1!$C$2:$C$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="38"/>
@@ -527,7 +527,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$39</c:f>
+              <c:f>sheet1!$D$2:$D$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="38"/>
@@ -660,7 +660,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$39</c:f>
+              <c:f>sheet1!$E$2:$E$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="38"/>
@@ -750,7 +750,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$39</c:f>
+              <c:f>sheet1!$F$2:$F$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="38"/>
@@ -877,7 +877,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$39</c:f>
+              <c:f>sheet1!$G$2:$G$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="38"/>
@@ -979,7 +979,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$39</c:f>
+              <c:f>sheet1!$H$2:$H$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="38"/>
@@ -1118,7 +1118,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$39</c:f>
+              <c:f>sheet1!$I$2:$I$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="38"/>
@@ -1241,7 +1241,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$39</c:f>
+              <c:f>sheet1!$J$2:$J$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="38"/>
@@ -2181,9 +2181,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2221,7 +2221,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2327,7 +2327,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2469,7 +2469,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2479,7 +2479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="T48" sqref="M40:T48"/>
     </sheetView>
   </sheetViews>

</xml_diff>